<commit_message>
Call agent after improvemnts
</commit_message>
<xml_diff>
--- a/cx_details.xlsx
+++ b/cx_details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Way to Denmark\Projects\Sinhala-call-center-assistant-for-Sri-Lanka-telecommunication-industry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F9207-C79C-4DB8-9EF1-4BB7B5248492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD233644-FD19-4F8B-8257-CC462E8167EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADC951EF-7AB2-41B9-BEF0-A96550E24845}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Customer_name</t>
   </si>
@@ -72,6 +72,36 @@
   </si>
   <si>
     <t>Pasan Sandeepa</t>
+  </si>
+  <si>
+    <t>20035301843V</t>
+  </si>
+  <si>
+    <t>19977593220V</t>
+  </si>
+  <si>
+    <t>20203162022V</t>
+  </si>
+  <si>
+    <t>20243492022V</t>
+  </si>
+  <si>
+    <t>19910751235V</t>
+  </si>
+  <si>
+    <t>19900323750V</t>
+  </si>
+  <si>
+    <t>19992251255V</t>
+  </si>
+  <si>
+    <t>20021215135V</t>
+  </si>
+  <si>
+    <t>20021151234V</t>
+  </si>
+  <si>
+    <t>Bill_amount</t>
   </si>
 </sst>
 </file>
@@ -107,8 +137,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,128 +480,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B976E571-7088-4E70-A31C-C33D3991F38B}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.44140625" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>20035301843</v>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C2">
         <v>732971526</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>19977593220</v>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
         <v>730044372</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>20203162022</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
         <v>733490579</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>20243492022</v>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C5">
         <v>734284591</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>19910751235</v>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C6">
         <v>730456566</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>19900323750</v>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C7">
         <v>731407363</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>19992251255</v>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C8">
         <v>738402409</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>6598</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>20021215135</v>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C9">
         <v>733822845</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>5396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>20021151234</v>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C10">
         <v>735486062</v>
+      </c>
+      <c r="D10">
+        <v>783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>